<commit_message>
fadeout Manager 수정 중
</commit_message>
<xml_diff>
--- a/hmm/dialogue/npc3.xlsx
+++ b/hmm/dialogue/npc3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sehui\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sehu\Desktop\Create with Code\ShoddyGame\hmm\dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313FEB35-3D94-4E1F-98D4-89C065504DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0FB928-7E24-4357-A3AA-19FCCFE322BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11505" xr2:uid="{15E8A521-AE4F-484D-8F3D-EA98EA3BD776}"/>
+    <workbookView xWindow="6465" yWindow="2700" windowWidth="18030" windowHeight="11460" xr2:uid="{15E8A521-AE4F-484D-8F3D-EA98EA3BD776}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7074A3B4-912B-4E30-B71E-C7E0A4929274}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>